<commit_message>
Added excel homework 19Feb2020
</commit_message>
<xml_diff>
--- a/module/monitor.xlsx
+++ b/module/monitor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimke\OneDrive\Documents\investment and trading\stocks and equity\sandbox\WealthAndFreedom\module\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="114_{76AE63C5-D422-42C8-B695-F6B1AA4E55A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{153C099D-3399-4EF6-A896-2DF4CDC165BB}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_A20D9A7F3841587EE94E24554E5DCE3A874662A7" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7EAC71B5-514E-4916-A522-8E5456FBB7F2}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="0" windowWidth="17445" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1365" yWindow="14175" windowWidth="17445" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
-  <si>
-    <t>2020-02-14</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
   <si>
     <t>2020-02-17</t>
   </si>
@@ -41,13 +38,7 @@
     <t>2020-02-18</t>
   </si>
   <si>
-    <t>5259</t>
-  </si>
-  <si>
-    <t>5073</t>
-  </si>
-  <si>
-    <t>9008</t>
+    <t>2020-02-19</t>
   </si>
   <si>
     <t>4723</t>
@@ -62,13 +53,10 @@
     <t>1538</t>
   </si>
   <si>
-    <t>EATECH</t>
-  </si>
-  <si>
-    <t>NAIM</t>
-  </si>
-  <si>
-    <t>OMESTI</t>
+    <t>9466</t>
+  </si>
+  <si>
+    <t>5286</t>
   </si>
   <si>
     <t>JAKS</t>
@@ -81,6 +69,12 @@
   </si>
   <si>
     <t>SYMLIFE</t>
+  </si>
+  <si>
+    <t>KKB</t>
+  </si>
+  <si>
+    <t>MI</t>
   </si>
 </sst>
 </file>
@@ -443,15 +437,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:I10"/>
+      <selection activeCell="A6" sqref="A6:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -489,69 +486,51 @@
         <v>0</v>
       </c>
       <c r="M1" s="1">
-        <v>1</v>
-      </c>
-      <c r="N1" s="1">
         <v>0</v>
       </c>
-      <c r="O1" s="1">
-        <v>1</v>
-      </c>
-      <c r="P1" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1581638400</v>
+        <v>1581897600</v>
       </c>
       <c r="B2">
+        <v>1581984000</v>
+      </c>
+      <c r="C2">
+        <v>1582070400</v>
+      </c>
+      <c r="D2">
         <v>1581897600</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>1581984000</v>
       </c>
-      <c r="D2">
-        <v>1581638400</v>
-      </c>
-      <c r="E2">
+      <c r="F2">
+        <v>1582070400</v>
+      </c>
+      <c r="G2">
         <v>1581897600</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>1581984000</v>
       </c>
-      <c r="G2">
-        <v>1581638400</v>
-      </c>
-      <c r="H2">
-        <v>1581897600</v>
-      </c>
       <c r="I2">
+        <v>1582070400</v>
+      </c>
+      <c r="J2">
         <v>1581984000</v>
       </c>
-      <c r="J2">
-        <v>1581897600</v>
-      </c>
       <c r="K2">
-        <v>1581984000</v>
+        <v>1582070400</v>
       </c>
       <c r="L2">
-        <v>1581897600</v>
+        <v>1582070400</v>
       </c>
       <c r="M2">
-        <v>1581984000</v>
-      </c>
-      <c r="N2">
-        <v>1581897600</v>
-      </c>
-      <c r="O2">
-        <v>1581984000</v>
-      </c>
-      <c r="P2">
-        <v>1581984000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1582070400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -586,22 +565,13 @@
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M3" t="s">
         <v>2</v>
       </c>
-      <c r="N3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -639,316 +609,253 @@
         <v>7</v>
       </c>
       <c r="M4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4" t="s">
         <v>8</v>
       </c>
-      <c r="O4" t="s">
-        <v>8</v>
-      </c>
-      <c r="P4" t="s">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
+      <c r="H5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>12</v>
       </c>
-      <c r="H5" t="s">
+      <c r="K5" t="s">
         <v>12</v>
       </c>
-      <c r="I5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>13</v>
-      </c>
-      <c r="K5" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" t="s">
-        <v>14</v>
       </c>
       <c r="M5" t="s">
         <v>14</v>
       </c>
-      <c r="N5" t="s">
-        <v>15</v>
-      </c>
-      <c r="O5" t="s">
-        <v>15</v>
-      </c>
-      <c r="P5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0.33</v>
+        <v>1.47</v>
       </c>
       <c r="B6">
-        <v>0.38</v>
+        <v>1.54</v>
       </c>
       <c r="C6">
-        <v>0.37</v>
+        <v>1.49</v>
       </c>
       <c r="D6">
-        <v>1.24</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="E6">
-        <v>1.36</v>
+        <v>0.74</v>
       </c>
       <c r="F6">
-        <v>1.33</v>
+        <v>0.71</v>
       </c>
       <c r="G6">
-        <v>0.55500000000000005</v>
+        <v>0.745</v>
       </c>
       <c r="H6">
-        <v>0.61</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="I6">
-        <v>0.60499999999999998</v>
+        <v>0.86499999999999999</v>
       </c>
       <c r="J6">
+        <v>0.4</v>
+      </c>
+      <c r="K6">
+        <v>0.45500000000000002</v>
+      </c>
+      <c r="L6">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="M6">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1.55</v>
+      </c>
+      <c r="B7">
+        <v>1.55</v>
+      </c>
+      <c r="C7">
+        <v>1.53</v>
+      </c>
+      <c r="D7">
+        <v>0.74</v>
+      </c>
+      <c r="E7">
+        <v>0.745</v>
+      </c>
+      <c r="F7">
+        <v>0.78</v>
+      </c>
+      <c r="G7">
+        <v>0.82</v>
+      </c>
+      <c r="H7">
+        <v>0.9</v>
+      </c>
+      <c r="I7">
+        <v>0.88</v>
+      </c>
+      <c r="J7">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="K7">
+        <v>0.46</v>
+      </c>
+      <c r="L7">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="M7">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1.46</v>
+      </c>
+      <c r="B8">
         <v>1.47</v>
       </c>
-      <c r="K6">
+      <c r="C8">
+        <v>1.49</v>
+      </c>
+      <c r="D8">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="E8">
+        <v>0.71</v>
+      </c>
+      <c r="F8">
+        <v>0.71</v>
+      </c>
+      <c r="G8">
+        <v>0.74</v>
+      </c>
+      <c r="H8">
+        <v>0.82</v>
+      </c>
+      <c r="I8">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="J8">
+        <v>0.4</v>
+      </c>
+      <c r="K8">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="L8">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="M8">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>1.54</v>
       </c>
-      <c r="L6">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="M6">
-        <v>0.74</v>
-      </c>
-      <c r="N6">
-        <v>0.745</v>
-      </c>
-      <c r="O6">
-        <v>0.82499999999999996</v>
-      </c>
-      <c r="P6">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="B7">
-        <v>0.39</v>
-      </c>
-      <c r="C7">
-        <v>0.37</v>
-      </c>
-      <c r="D7">
-        <v>1.37</v>
-      </c>
-      <c r="E7">
-        <v>1.41</v>
-      </c>
-      <c r="F7">
-        <v>1.36</v>
-      </c>
-      <c r="G7">
-        <v>0.61</v>
-      </c>
-      <c r="H7">
-        <v>0.63</v>
-      </c>
-      <c r="I7">
-        <v>0.61</v>
-      </c>
-      <c r="J7">
-        <v>1.55</v>
-      </c>
-      <c r="K7">
-        <v>1.55</v>
-      </c>
-      <c r="L7">
-        <v>0.74</v>
-      </c>
-      <c r="M7">
-        <v>0.745</v>
-      </c>
-      <c r="N7">
-        <v>0.82</v>
-      </c>
-      <c r="O7">
-        <v>0.9</v>
-      </c>
-      <c r="P7">
-        <v>0.46500000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0.33</v>
-      </c>
-      <c r="B8">
-        <v>0.36499999999999999</v>
-      </c>
-      <c r="C8">
-        <v>0.35</v>
-      </c>
-      <c r="D8">
-        <v>1.24</v>
-      </c>
-      <c r="E8">
-        <v>1.33</v>
-      </c>
-      <c r="F8">
-        <v>1.31</v>
-      </c>
-      <c r="G8">
-        <v>0.55500000000000005</v>
-      </c>
-      <c r="H8">
-        <v>0.58499999999999996</v>
-      </c>
-      <c r="I8">
-        <v>0.57499999999999996</v>
-      </c>
-      <c r="J8">
-        <v>1.46</v>
-      </c>
-      <c r="K8">
-        <v>1.47</v>
-      </c>
-      <c r="L8">
-        <v>0.67500000000000004</v>
-      </c>
-      <c r="M8">
-        <v>0.71</v>
-      </c>
-      <c r="N8">
-        <v>0.74</v>
-      </c>
-      <c r="O8">
-        <v>0.82</v>
-      </c>
-      <c r="P8">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0.38500000000000001</v>
-      </c>
       <c r="B9">
-        <v>0.37</v>
+        <v>1.49</v>
       </c>
       <c r="C9">
-        <v>0.35</v>
+        <v>1.52</v>
       </c>
       <c r="D9">
-        <v>1.36</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="E9">
-        <v>1.34</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="F9">
-        <v>1.33</v>
+        <v>0.77500000000000002</v>
       </c>
       <c r="G9">
-        <v>0.6</v>
+        <v>0.81</v>
       </c>
       <c r="H9">
-        <v>0.6</v>
+        <v>0.86</v>
       </c>
       <c r="I9">
-        <v>0.57999999999999996</v>
+        <v>0.875</v>
       </c>
       <c r="J9">
-        <v>1.54</v>
+        <v>0.46</v>
       </c>
       <c r="K9">
-        <v>1.49</v>
+        <v>0.45</v>
       </c>
       <c r="L9">
-        <v>0.73499999999999999</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="M9">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="N9">
-        <v>0.81</v>
-      </c>
-      <c r="O9">
-        <v>0.86</v>
-      </c>
-      <c r="P9">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>83977</v>
+        <v>252788</v>
       </c>
       <c r="B10">
-        <v>49244</v>
+        <v>151765</v>
       </c>
       <c r="C10">
-        <v>34472</v>
+        <v>91240</v>
       </c>
       <c r="D10">
-        <v>236252</v>
+        <v>139048</v>
       </c>
       <c r="E10">
-        <v>98265</v>
+        <v>38926</v>
       </c>
       <c r="F10">
-        <v>30101</v>
+        <v>112753</v>
       </c>
       <c r="G10">
-        <v>121218</v>
+        <v>157314</v>
       </c>
       <c r="H10">
-        <v>109651</v>
+        <v>516909</v>
       </c>
       <c r="I10">
-        <v>29570</v>
+        <v>173554</v>
       </c>
       <c r="J10">
-        <v>252788</v>
+        <v>56745</v>
       </c>
       <c r="K10">
-        <v>151765</v>
+        <v>14960</v>
       </c>
       <c r="L10">
-        <v>139048</v>
+        <v>38086</v>
       </c>
       <c r="M10">
-        <v>38926</v>
-      </c>
-      <c r="N10">
-        <v>157314</v>
-      </c>
-      <c r="O10">
-        <v>516909</v>
-      </c>
-      <c r="P10">
-        <v>56745</v>
+        <v>77447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>